<commit_message>
responsive viewing - wip
</commit_message>
<xml_diff>
--- a/stories/userstories.xlsx
+++ b/stories/userstories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb_000\CI_InteractiveFrontend\CI_InteractiveFrontend\stories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fizzb\Desktop\projects\CI\CI_InteractiveFrontend\CI_InteractiveFrontend\stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{759FB661-B20C-47BF-B288-B4A0CBA86DDD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2FF43A73-01A8-4E62-8695-330AA24C1111}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9375" xr2:uid="{C91606FE-5190-4451-B3A8-F761A2188AA6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{C91606FE-5190-4451-B3A8-F761A2188AA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>As a webpage administrator</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>I present the data visualisation clearly, so that the visitos are not overwhelmed by the webpage.</t>
+  </si>
+  <si>
+    <t>2 personas</t>
+  </si>
+  <si>
+    <t>invent users; give name,age, bg; backstory; technologically savvy or not; purpose of visit</t>
   </si>
 </sst>
 </file>
@@ -78,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -98,9 +110,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C4D366-96E4-4420-9A28-5E9976D934B0}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +482,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>